<commit_message>
add configuration of base metrics and derived metrics.
</commit_message>
<xml_diff>
--- a/doc/模拟指标定义.xlsx
+++ b/doc/模拟指标定义.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\metric-sys\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741458E8-EE41-4969-8893-5AD2EB1704C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1932A27-6D41-4BB5-9E47-A497D59D7F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="5950" windowWidth="15360" windowHeight="9670" xr2:uid="{AED58BA3-94E0-4E10-9A90-6B6229FA4916}"/>
+    <workbookView xWindow="8080" yWindow="3630" windowWidth="28800" windowHeight="15460" xr2:uid="{AED58BA3-94E0-4E10-9A90-6B6229FA4916}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>指标名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,113 +64,191 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>核酸检测人次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b000000011</t>
+  </si>
+  <si>
+    <t>统计各行政区域在不同日期的核酸检测人次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>健康异常人数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各行政区域在不同日期的健康异常人次（体温&gt;37，或有咳嗽、胸闷症状）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大专学历以上人口数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各日期大专学历以上人口数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>累计新冠患者数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b000000002</t>
+  </si>
+  <si>
+    <t>统计各日期累计新冠患者数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b000000020</t>
+  </si>
+  <si>
+    <t>就业人数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期、行政区划、行业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各日期、行政区划和行业的就业人数（按居住地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小微企业数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中型企业数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b000000022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各日期、行政区划和行业的小微企业数量（按企业注册地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各日期、行政区划和行业的中型企业数量（按企业注册地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大型企业数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b000000023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各日期、行政区划和行业的大型企业数量（按企业注册地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>企业净利润</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b000000024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各日期、行政区划和行业的企业净利润（按企业注册地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指标类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础指标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>衍生指标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>健康异常人口比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b000000012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>b000000010</t>
-  </si>
-  <si>
-    <t>核酸检测人次</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b000000011</t>
-  </si>
-  <si>
-    <t>统计各行政区域在不同日期的核酸检测人次</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>健康异常人数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b000000012</t>
-  </si>
-  <si>
-    <t>统计各行政区域在不同日期的健康异常人次（体温&gt;37，或有咳嗽、胸闷症状）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大专学历以上人口数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>统计各日期大专学历以上人口数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>累计新冠患者数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b000000002</t>
-  </si>
-  <si>
-    <t>统计各日期累计新冠患者数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b000000020</t>
-  </si>
-  <si>
-    <t>就业人数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期、行政区划、行业</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>统计各日期、行政区划和行业的就业人数（按居住地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d000000011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期、行政区划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各行政区域内不同日期健康异常人口比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增新冠患者数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b000000003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各日期新增新冠患者数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新冠患者占人口比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d000000001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计不同日期累计新冠患者数量占总人口比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中小企业数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>b000000021</t>
-  </si>
-  <si>
-    <t>小微企业数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中型企业数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b000000022</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>统计各日期、行政区划和行业的小微企业数量（按企业注册地区统计）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>统计各日期、行政区划和行业的中型企业数量（按企业注册地区统计）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大型企业数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b000000023</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>统计各日期、行政区划和行业的大型企业数量（按企业注册地区统计）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>企业净利润</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b000000024</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>统计各日期、行政区划和行业的企业净利润（按企业注册地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d000000021</t>
+  </si>
+  <si>
+    <t>统计各日期、行政区划和行业的中小型企业数量（按企业注册地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中小企业数量占比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计各日期、行政区划和行业的中小型企业数量占比（按企业注册地区统计）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d000000022</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,176 +622,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A07F916-20DE-4B40-88D9-0E2EF8861501}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>